<commit_message>
Web App, maybe mistakes, sending emails when there is court decision, but very very slow
</commit_message>
<xml_diff>
--- a/SOLON_INPUT.xlsx
+++ b/SOLON_INPUT.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Πελάτης</t>
   </si>
@@ -37,100 +37,94 @@
     <t>Αποτέλεσμα Συζήτησης</t>
   </si>
   <si>
-    <t>ΑΝΤΩΝΙΟΥ ΑΝΔΡΕΑΣ</t>
+    <t>ΜΠΕΓΙΑΣ ΘΕΟΔΩΡΟΣ</t>
+  </si>
+  <si>
+    <t>ΠΡΩΤΟΔΙΚΕΙΟ ΑΘΗΝΩΝ</t>
+  </si>
+  <si>
+    <t>ΠΕΤΥΧΑΚΗΣ ΜΙΧΑΛΗΣ</t>
+  </si>
+  <si>
+    <t>ΚΑΡΑΤΖΑΦΕΡΗΣ ΒΑΣΙΛΗΣ</t>
+  </si>
+  <si>
+    <t>ΕΦΕΤΕΙΟ ΑΘΗΝΩΝ</t>
+  </si>
+  <si>
+    <t>ΜΠΑΣΔΕΚΗΣ ΚΩΣΤΑΣ</t>
+  </si>
+  <si>
+    <t>ΣΕΪΜΕΝΗΣ ΓΙΑΝΝΗΣ1</t>
+  </si>
+  <si>
+    <t>ΣΕΪΜΕΝΗΣ ΓΙΑΝΝΗΣ2</t>
+  </si>
+  <si>
+    <t>ΤΣΙΡΟΠΟΥΛΟΥ ΣΤΑΜΑΤΙΑ</t>
+  </si>
+  <si>
+    <t>ΒΑΚΑΛΟΠΟΥΛΟΥ ΔΕΔΔΗΕ</t>
+  </si>
+  <si>
+    <t>ΚΑΚΑΛΗΣ ΚΩΣΤΑΣ</t>
+  </si>
+  <si>
+    <t>ΒΑΚΑΛΟΠΟΥΛΟΥ ΧΕΙΡΔ</t>
+  </si>
+  <si>
+    <t>ΕΙΡΗΝΟΔΙΚΕΙΟ ΧΑΛΚΙΔΑΣ</t>
+  </si>
+  <si>
+    <t>ΜΑΝΤΖΑΡΗ</t>
+  </si>
+  <si>
+    <t>ΓΙΑΝΝΑΚΟΠΟΥΛΟΥ</t>
+  </si>
+  <si>
+    <t>ΕΙΡΗΝΟΔΙΚΕΙΟ ΚΡΩΠΙΑΣ</t>
+  </si>
+  <si>
+    <t>ΣΕΡΕΤΗ ΓΙΩΤΑ</t>
+  </si>
+  <si>
+    <t>ΓΟΥΛΑΣ ΠΑΝΟΣ</t>
+  </si>
+  <si>
+    <t>ΠΑΥΛΗ ΕΥΑΓΓΕΛΙΑ</t>
+  </si>
+  <si>
+    <t>ΜΑΤΣΙΩΤΑΣ</t>
+  </si>
+  <si>
+    <t>ΚΑΣΙΔΑΚΗ</t>
+  </si>
+  <si>
+    <t>ΣΠΥΡΟΠΟΥΛΟΣ</t>
+  </si>
+  <si>
+    <t>ΜΑΡΚΟΥΛΗΣ</t>
+  </si>
+  <si>
+    <t>ΚΟΥΤΣΙΟΣ</t>
+  </si>
+  <si>
+    <t>ΚΥΡΙΑΖΗΣ</t>
+  </si>
+  <si>
+    <t>ΛΑΜΠΡΟΠΟΥΛΟΣ</t>
+  </si>
+  <si>
+    <t>ΓΚΑΝΤΩΝΑ ΓΙΩΤΑ</t>
   </si>
   <si>
     <t>ΕΙΡΗΝΟΔΙΚΕΙΟ ΑΘΗΝΩΝ</t>
   </si>
   <si>
-    <t>ΜΠΕΓΙΑΣ ΘΕΟΔΩΡΟΣ</t>
-  </si>
-  <si>
-    <t>ΠΡΩΤΟΔΙΚΕΙΟ ΑΘΗΝΩΝ</t>
-  </si>
-  <si>
-    <t>ΠΕΤΥΧΑΚΗΣ ΜΙΧΑΛΗΣ</t>
-  </si>
-  <si>
-    <t>ΚΑΡΑΤΖΑΦΕΡΗΣ ΒΑΣΙΛΗΣ</t>
-  </si>
-  <si>
-    <t>ΕΦΕΤΕΙΟ ΑΘΗΝΩΝ</t>
-  </si>
-  <si>
-    <t>ΜΠΑΣΔΕΚΗΣ ΚΩΣΤΑΣ</t>
-  </si>
-  <si>
-    <t>ΣΕΪΜΕΝΗΣ ΓΙΑΝΝΗΣ1</t>
-  </si>
-  <si>
-    <t>ΣΕΪΜΕΝΗΣ ΓΙΑΝΝΗΣ2</t>
-  </si>
-  <si>
-    <t>ΤΣΙΡΟΠΟΥΛΟΥ ΣΤΑΜΑΤΙΑ</t>
-  </si>
-  <si>
-    <t>ΒΑΚΑΛΟΠΟΥΛΟΥ ΔΕΔΔΗΕ</t>
-  </si>
-  <si>
-    <t>ΚΑΚΑΛΗΣ ΚΩΣΤΑΣ</t>
-  </si>
-  <si>
-    <t>ΒΑΚΑΛΟΠΟΥΛΟΥ ΧΕΙΡΔ</t>
-  </si>
-  <si>
-    <t>ΕΙΡΗΝΟΔΙΚΕΙΟ ΧΑΛΚΙΔΑΣ</t>
-  </si>
-  <si>
-    <t>ΜΑΝΤΖΑΡΗ</t>
-  </si>
-  <si>
-    <t>ΓΙΑΝΝΑΚΟΠΟΥΛΟΥ</t>
-  </si>
-  <si>
-    <t>ΕΙΡΗΝΟΔΙΚΕΙΟ ΚΡΩΠΙΑΣ</t>
-  </si>
-  <si>
-    <t>ΣΕΡΕΤΗ ΓΙΩΤΑ</t>
-  </si>
-  <si>
-    <t>ΓΟΥΛΑΣ ΠΑΝΟΣ</t>
-  </si>
-  <si>
-    <t>ΠΑΥΛΗ ΕΥΑΓΓΕΛΙΑ</t>
-  </si>
-  <si>
-    <t>ΜΑΤΣΙΩΤΑΣ</t>
-  </si>
-  <si>
-    <t>ΚΑΣΙΔΑΚΗ</t>
-  </si>
-  <si>
-    <t>ΣΠΥΡΟΠΟΥΛΟΣ</t>
-  </si>
-  <si>
-    <t>ΜΑΡΚΟΥΛΗΣ</t>
-  </si>
-  <si>
-    <t>ΚΟΥΤΣΙΟΣ</t>
-  </si>
-  <si>
-    <t>ΚΥΡΙΑΖΗΣ</t>
-  </si>
-  <si>
-    <t>ΛΑΜΠΡΟΠΟΥΛΟΣ</t>
-  </si>
-  <si>
-    <t>ΓΚΑΝΤΩΝΑ ΓΙΩΤΑ</t>
-  </si>
-  <si>
     <t>ΠΕΡΓΑΝΤΗΣ ΣΤΕΛΙΟΣ Euro</t>
   </si>
   <si>
-    <t>ΛΙΖΟΣ</t>
-  </si>
-  <si>
-    <t>ΓΑΓΚΑ</t>
+    <t>ΛΙΖΟΣ ΚΩΣΤΑΣ</t>
   </si>
   <si>
     <t>ΠΑΠΑΔΑΣΚΑΛΟΠΟΥΛΟΥ</t>
@@ -151,9 +145,6 @@
     <t>ΚΟΥΤΣΟΥΜΠΑΣ</t>
   </si>
   <si>
-    <t>ΛΙΑΚΟΥΤΣΗΣ</t>
-  </si>
-  <si>
     <t>ΜΑΘΙΟΥ</t>
   </si>
   <si>
@@ -169,15 +160,6 @@
     <t>ΜΑΡΓΑΡΙΤΗ</t>
   </si>
   <si>
-    <t>ΣΤΑΥΡΟΥΛΑΚΗ ΒΑΣΩ ΑΓΩΓΗ</t>
-  </si>
-  <si>
-    <t>ΕΙΡΗΝΟΔΙΚΕΙΟ ΚΑΛΛΙΘΕΑΣ</t>
-  </si>
-  <si>
-    <t>ΣΤΑΥΡΟΥΛΑΚΗ ΒΑΣΩ ΑΝΤΑΓΩΓΗ</t>
-  </si>
-  <si>
     <t>ΤΖΑΡΑ vs ΕΤΕ</t>
   </si>
   <si>
@@ -199,13 +181,7 @@
     <t>ΤΣΕΒΗΣ</t>
   </si>
   <si>
-    <t>ΚΟΥΡΗΣ ΣΠΥΡΟΣ</t>
-  </si>
-  <si>
-    <t>ΔΟΚΙΜΗ1</t>
-  </si>
-  <si>
-    <t>ΔΟΚΙΜΗ2</t>
+    <t>ΔΟΚΙΜΗ RUN OF SOLON_AUTO</t>
   </si>
 </sst>
 </file>
@@ -1461,7 +1437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -1509,10 +1485,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="5">
-        <v>19684</v>
+        <v>128639</v>
       </c>
       <c r="D2" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1524,10 +1500,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="9">
-        <v>128639</v>
+        <v>103819</v>
       </c>
       <c r="D3" s="9">
         <v>2024</v>
@@ -1539,13 +1515,13 @@
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="8">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="8">
-        <v>11</v>
-      </c>
       <c r="C4" s="9">
-        <v>103819</v>
+        <v>8155</v>
       </c>
       <c r="D4" s="9">
         <v>2024</v>
@@ -1560,10 +1536,10 @@
         <v>13</v>
       </c>
       <c r="B5" t="s" s="8">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="9">
-        <v>8155</v>
+        <v>104339</v>
       </c>
       <c r="D5" s="9">
         <v>2024</v>
@@ -1575,13 +1551,13 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9">
-        <v>104339</v>
+        <v>8154</v>
       </c>
       <c r="D6" s="9">
         <v>2024</v>
@@ -1593,16 +1569,16 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s" s="8">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C7" s="9">
-        <v>8154</v>
+        <v>154164</v>
       </c>
       <c r="D7" s="9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -1611,16 +1587,16 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="9">
-        <v>154164</v>
+        <v>45359</v>
       </c>
       <c r="D8" s="9">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -1629,13 +1605,13 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="9">
-        <v>45359</v>
+        <v>119548</v>
       </c>
       <c r="D9" s="9">
         <v>2022</v>
@@ -1647,13 +1623,13 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="9">
-        <v>119548</v>
+        <v>121656</v>
       </c>
       <c r="D10" s="9">
         <v>2022</v>
@@ -1665,16 +1641,16 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="8">
-        <v>11</v>
-      </c>
       <c r="C11" s="9">
-        <v>121656</v>
+        <v>863</v>
       </c>
       <c r="D11" s="9">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1686,13 +1662,13 @@
         <v>21</v>
       </c>
       <c r="B12" t="s" s="8">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C12" s="9">
-        <v>863</v>
+        <v>35606</v>
       </c>
       <c r="D12" s="9">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1701,16 +1677,16 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s" s="8">
         <v>23</v>
       </c>
-      <c r="B13" t="s" s="8">
-        <v>11</v>
-      </c>
       <c r="C13" s="9">
-        <v>35606</v>
+        <v>3590</v>
       </c>
       <c r="D13" s="9">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1722,13 +1698,13 @@
         <v>24</v>
       </c>
       <c r="B14" t="s" s="8">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C14" s="9">
-        <v>3590</v>
+        <v>37388</v>
       </c>
       <c r="D14" s="9">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1737,16 +1713,16 @@
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" s="9">
-        <v>37388</v>
+        <v>83768</v>
       </c>
       <c r="D15" s="9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1755,13 +1731,13 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="9">
-        <v>83768</v>
+        <v>83109</v>
       </c>
       <c r="D16" s="9">
         <v>2025</v>
@@ -1773,16 +1749,16 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="7">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="9">
-        <v>83109</v>
+        <v>127165</v>
       </c>
       <c r="D17" s="9">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -1791,13 +1767,13 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" s="9">
-        <v>127165</v>
+        <v>128639</v>
       </c>
       <c r="D18" s="9">
         <v>2022</v>
@@ -1809,16 +1785,16 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" s="9">
-        <v>128639</v>
+        <v>118721</v>
       </c>
       <c r="D19" s="9">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -1827,16 +1803,16 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" s="9">
-        <v>118721</v>
+        <v>2627</v>
       </c>
       <c r="D20" s="9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1845,13 +1821,13 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="9">
-        <v>2627</v>
+        <v>98797</v>
       </c>
       <c r="D21" s="9">
         <v>2025</v>
@@ -1863,13 +1839,13 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="7">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s" s="8">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C22" s="9">
-        <v>98797</v>
+        <v>115245</v>
       </c>
       <c r="D22" s="9">
         <v>2025</v>
@@ -1881,13 +1857,13 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C23" s="9">
-        <v>115245</v>
+        <v>194682</v>
       </c>
       <c r="D23" s="9">
         <v>2025</v>
@@ -1899,16 +1875,16 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="B24" t="s" s="8">
-        <v>11</v>
-      </c>
       <c r="C24" s="9">
-        <v>194682</v>
+        <v>46666</v>
       </c>
       <c r="D24" s="9">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1923,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="9">
-        <v>46666</v>
+        <v>44181</v>
       </c>
       <c r="D25" s="9">
         <v>2023</v>
@@ -1938,10 +1914,10 @@
         <v>37</v>
       </c>
       <c r="B26" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" s="9">
-        <v>44181</v>
+        <v>16304</v>
       </c>
       <c r="D26" s="9">
         <v>2023</v>
@@ -1956,13 +1932,13 @@
         <v>38</v>
       </c>
       <c r="B27" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27" s="9">
-        <v>16304</v>
+        <v>200457</v>
       </c>
       <c r="D27" s="9">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -1974,10 +1950,10 @@
         <v>39</v>
       </c>
       <c r="B28" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C28" s="9">
-        <v>50290</v>
+        <v>499</v>
       </c>
       <c r="D28" s="9">
         <v>2024</v>
@@ -1992,13 +1968,13 @@
         <v>40</v>
       </c>
       <c r="B29" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C29" s="9">
-        <v>200457</v>
+        <v>66563</v>
       </c>
       <c r="D29" s="9">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -2010,10 +1986,10 @@
         <v>41</v>
       </c>
       <c r="B30" t="s" s="8">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C30" s="9">
-        <v>499</v>
+        <v>7078</v>
       </c>
       <c r="D30" s="9">
         <v>2024</v>
@@ -2025,16 +2001,16 @@
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31" s="9">
-        <v>66563</v>
+        <v>92174</v>
       </c>
       <c r="D31" s="9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -2043,16 +2019,16 @@
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s" s="8">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C32" s="9">
-        <v>7078</v>
+        <v>52527</v>
       </c>
       <c r="D32" s="9">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -2064,13 +2040,13 @@
         <v>45</v>
       </c>
       <c r="B33" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C33" s="9">
-        <v>92174</v>
+        <v>8973</v>
       </c>
       <c r="D33" s="9">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -2082,10 +2058,10 @@
         <v>46</v>
       </c>
       <c r="B34" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C34" s="9">
-        <v>87931</v>
+        <v>39008</v>
       </c>
       <c r="D34" s="9">
         <v>2023</v>
@@ -2100,13 +2076,13 @@
         <v>47</v>
       </c>
       <c r="B35" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C35" s="9">
-        <v>52527</v>
+        <v>11108</v>
       </c>
       <c r="D35" s="9">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -2118,13 +2094,13 @@
         <v>48</v>
       </c>
       <c r="B36" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C36" s="9">
-        <v>8973</v>
+        <v>132783</v>
       </c>
       <c r="D36" s="9">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -2136,13 +2112,13 @@
         <v>49</v>
       </c>
       <c r="B37" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C37" s="9">
-        <v>39008</v>
+        <v>25898</v>
       </c>
       <c r="D37" s="9">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -2154,13 +2130,13 @@
         <v>50</v>
       </c>
       <c r="B38" t="s" s="8">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C38" s="9">
-        <v>11108</v>
+        <v>18012</v>
       </c>
       <c r="D38" s="9">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -2172,13 +2148,13 @@
         <v>51</v>
       </c>
       <c r="B39" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39" s="9">
-        <v>132783</v>
+        <v>136764</v>
       </c>
       <c r="D39" s="9">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -2190,10 +2166,10 @@
         <v>52</v>
       </c>
       <c r="B40" t="s" s="8">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C40" s="9">
-        <v>1405</v>
+        <v>63010</v>
       </c>
       <c r="D40" s="9">
         <v>2023</v>
@@ -2205,16 +2181,16 @@
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="7">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s" s="8">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C41" s="9">
-        <v>35295</v>
+        <v>13697</v>
       </c>
       <c r="D41" s="9">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -2223,13 +2199,13 @@
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="7">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C42" s="9">
-        <v>25898</v>
+        <v>128690</v>
       </c>
       <c r="D42" s="9">
         <v>2024</v>
@@ -2241,13 +2217,13 @@
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="7">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s" s="8">
         <v>9</v>
       </c>
       <c r="C43" s="9">
-        <v>18012</v>
+        <v>129983</v>
       </c>
       <c r="D43" s="9">
         <v>2024</v>
@@ -2259,16 +2235,16 @@
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="7">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C44" s="9">
-        <v>136764</v>
+        <v>70927</v>
       </c>
       <c r="D44" s="9">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -2276,126 +2252,70 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="B45" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="C45" s="9">
-        <v>63010</v>
-      </c>
-      <c r="D45" s="9">
-        <v>2023</v>
-      </c>
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="B46" t="s" s="8">
-        <v>44</v>
-      </c>
-      <c r="C46" s="9">
-        <v>13697</v>
-      </c>
-      <c r="D46" s="9">
-        <v>2024</v>
-      </c>
+      <c r="A46" s="11"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" t="s" s="7">
-        <v>60</v>
-      </c>
-      <c r="B47" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C47" s="9">
-        <v>128690</v>
-      </c>
-      <c r="D47" s="9">
-        <v>2024</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" t="s" s="7">
-        <v>61</v>
-      </c>
-      <c r="B48" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C48" s="9">
-        <v>129983</v>
-      </c>
-      <c r="D48" s="9">
-        <v>2024</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="B49" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C49" s="9">
-        <v>132679</v>
-      </c>
-      <c r="D49" s="9">
-        <v>2024</v>
-      </c>
+      <c r="A49" s="11"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" t="s" s="7">
-        <v>63</v>
-      </c>
-      <c r="B50" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="C50" s="9">
-        <v>19684</v>
-      </c>
-      <c r="D50" s="9">
-        <v>2023</v>
-      </c>
+      <c r="A50" s="11"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="B51" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C51" s="9">
-        <v>70927</v>
-      </c>
-      <c r="D51" s="9">
-        <v>2025</v>
-      </c>
+      <c r="A51" s="11"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
@@ -2471,76 +2391,6 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
     </row>
-    <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" s="11"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
-    </row>
-    <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" s="11"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-    </row>
-    <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" s="11"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-    </row>
-    <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" s="11"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-    </row>
-    <row r="63" ht="20.05" customHeight="1">
-      <c r="A63" s="11"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-    </row>
-    <row r="64" ht="20.05" customHeight="1">
-      <c r="A64" s="11"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-    </row>
-    <row r="65" ht="20.05" customHeight="1">
-      <c r="A65" s="11"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
-    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>